<commit_message>
helpline eval controlled by cpu load
</commit_message>
<xml_diff>
--- a/jadex-applications-micro/EvalUni_SSPvsAwarenessDynservices.xlsx
+++ b/jadex-applications-micro/EvalUni_SSPvsAwarenessDynservices.xlsx
@@ -53,7 +53,7 @@
     <t>Settings: '-spcnt 3 -platformcnt -10 -personcnt 1'</t>
   </si>
   <si>
-    <t>Settings: '-spcnt 0 -platformcnt -10 -personcnt 1'</t>
+    <t>Settings: '-spcnt 0 -platformcnt -1 -personcnt 1'</t>
   </si>
 </sst>
 </file>
@@ -124,38 +124,16 @@
   <c:chart>
     <c:title>
       <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="de-DE"/>
-              <a:t>SP: Settings: '-spcnt 3 -platformcnt -1 -personcnt 0'</a:t>
-            </a:r>
-          </a:p>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="de-DE"/>
-              <a:t>Awa: Settings: '-spcnt 0 -platformcnt -1 -personcnt 0'</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
+        <c:strRef>
+          <c:f>Tabelle1!$R$3</c:f>
+          <c:strCache>
+            <c:ptCount val="1"/>
+            <c:pt idx="0">
+              <c:v>Settings: '-spcnt 3 -platformcnt -10 -personcnt 1'
+Settings: '-spcnt 0 -platformcnt -1 -personcnt 1'</c:v>
+            </c:pt>
+          </c:strCache>
+        </c:strRef>
       </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
@@ -1219,88 +1197,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
                 <c:pt idx="0">
-                  <c:v>285.55192799999998</c:v>
+                  <c:v>13.044903</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>47.591636000000001</c:v>
+                  <c:v>12.740627999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>39.881211999999998</c:v>
+                  <c:v>10.611908</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>61.841264000000002</c:v>
+                  <c:v>13.360951</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50.772641999999998</c:v>
+                  <c:v>14.165108</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>50.579752999999997</c:v>
+                  <c:v>15.806323000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>25.322779000000001</c:v>
+                  <c:v>12.866201999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>34.907456000000003</c:v>
+                  <c:v>12.800094</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>52.141579</c:v>
+                  <c:v>22.639842000000002</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>65.303605000000005</c:v>
+                  <c:v>18.587063000000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>100.469453</c:v>
+                  <c:v>15.831378000000001</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>49.055357999999998</c:v>
+                  <c:v>24.456137999999999</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>63.487310999999998</c:v>
+                  <c:v>18.024093000000001</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>128.539466</c:v>
+                  <c:v>22.389600999999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>141.32024100000001</c:v>
+                  <c:v>36.025244999999998</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>191.37505999999999</c:v>
+                  <c:v>39.111165</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>326.80600199999998</c:v>
+                  <c:v>22.942609999999998</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>366.15835399999997</c:v>
+                  <c:v>37.693326999999996</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>440.23281900000001</c:v>
+                  <c:v>57.586238999999999</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1087.4390390000001</c:v>
+                  <c:v>74.960425999999998</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>118.36072900000001</c:v>
+                  <c:v>263.34917899999999</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1518.6257009999999</c:v>
+                  <c:v>102.681488</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>839.83098299999995</c:v>
+                  <c:v>214.71129500000001</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>566.17356700000005</c:v>
+                  <c:v>370.14774299999999</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>704.65662199999997</c:v>
+                  <c:v>51.258637999999998</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>3103.9163990000002</c:v>
+                  <c:v>402.48123399999997</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>8506.0341929999995</c:v>
+                  <c:v>2347.0795589999998</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>13880.508502000001</c:v>
+                  <c:v>74.959519999999998</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>144.595731</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>62.140711000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1654,88 +1638,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
                 <c:pt idx="0">
-                  <c:v>1667.923211</c:v>
+                  <c:v>223.06951100000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1376.4696080000001</c:v>
+                  <c:v>230.943242</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1241.979867</c:v>
+                  <c:v>217.69246899999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1553.185414</c:v>
+                  <c:v>228.125978</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1274.1425039999999</c:v>
+                  <c:v>263.494978</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1225.971297</c:v>
+                  <c:v>240.38362900000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1400.326251</c:v>
+                  <c:v>263.86596400000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1317.315204</c:v>
+                  <c:v>241.20740599999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1232.531933</c:v>
+                  <c:v>254.00538800000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1241.9451529999999</c:v>
+                  <c:v>259.46514000000002</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1244.0162190000001</c:v>
+                  <c:v>256.45106199999998</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1260.781855</c:v>
+                  <c:v>373.45311600000002</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1530.580285</c:v>
+                  <c:v>298.67139100000003</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1709.87247</c:v>
+                  <c:v>498.03247299999998</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1713.2188960000001</c:v>
+                  <c:v>363.73079100000001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1299.587839</c:v>
+                  <c:v>335.15546399999999</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1657.974794</c:v>
+                  <c:v>292.869933</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1486.057665</c:v>
+                  <c:v>288.34444000000002</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2151.6544370000001</c:v>
+                  <c:v>716.17199800000003</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2038.5303859999999</c:v>
+                  <c:v>333.04666600000002</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2832.1848540000001</c:v>
+                  <c:v>1439.6864519999999</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2279.2279490000001</c:v>
+                  <c:v>2397.771002</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>3318.2705930000002</c:v>
+                  <c:v>1876.7702609999999</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>3658.1806630000001</c:v>
+                  <c:v>3361.3008140000002</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>4264.5928439999998</c:v>
+                  <c:v>718.56665699999996</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>6556.0165630000001</c:v>
+                  <c:v>2124.5168720000001</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>6496.5461109999997</c:v>
+                  <c:v>4635.1813030000003</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>12842.04996</c:v>
+                  <c:v>5104.0190309999998</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>7838.3213779999996</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>9029.3701259999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2920,15 +2910,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N203"/>
+  <dimension ref="A1:R203"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:N133"/>
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -2972,7 +2962,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>3</v>
       </c>
@@ -3001,16 +2991,16 @@
         <v>10</v>
       </c>
       <c r="K2">
-        <v>285.55192799999998</v>
+        <v>13.044903</v>
       </c>
       <c r="L2">
-        <v>1667.923211</v>
+        <v>223.06951100000001</v>
       </c>
       <c r="M2">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
@@ -3039,16 +3029,21 @@
         <v>20</v>
       </c>
       <c r="K3">
-        <v>47.591636000000001</v>
+        <v>12.740627999999999</v>
       </c>
       <c r="L3">
-        <v>1376.4696080000001</v>
+        <v>230.943242</v>
       </c>
       <c r="M3">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="R3" t="str">
+        <f>G1&amp;CHAR(10)&amp;N1</f>
+        <v>Settings: '-spcnt 3 -platformcnt -10 -personcnt 1'
+Settings: '-spcnt 0 -platformcnt -1 -personcnt 1'</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3077,16 +3072,16 @@
         <v>30</v>
       </c>
       <c r="K4">
-        <v>39.881211999999998</v>
+        <v>10.611908</v>
       </c>
       <c r="L4">
-        <v>1241.979867</v>
+        <v>217.69246899999999</v>
       </c>
       <c r="M4">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -3115,16 +3110,16 @@
         <v>40</v>
       </c>
       <c r="K5">
-        <v>61.841264000000002</v>
+        <v>13.360951</v>
       </c>
       <c r="L5">
-        <v>1553.185414</v>
+        <v>228.125978</v>
       </c>
       <c r="M5">
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -3153,16 +3148,16 @@
         <v>50</v>
       </c>
       <c r="K6">
-        <v>50.772641999999998</v>
+        <v>14.165108</v>
       </c>
       <c r="L6">
-        <v>1274.1425039999999</v>
+        <v>263.494978</v>
       </c>
       <c r="M6">
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -3191,16 +3186,16 @@
         <v>60</v>
       </c>
       <c r="K7">
-        <v>50.579752999999997</v>
+        <v>15.806323000000001</v>
       </c>
       <c r="L7">
-        <v>1225.971297</v>
+        <v>240.38362900000001</v>
       </c>
       <c r="M7">
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3</v>
       </c>
@@ -3229,16 +3224,16 @@
         <v>70</v>
       </c>
       <c r="K8">
-        <v>25.322779000000001</v>
+        <v>12.866201999999999</v>
       </c>
       <c r="L8">
-        <v>1400.326251</v>
+        <v>263.86596400000002</v>
       </c>
       <c r="M8">
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3</v>
       </c>
@@ -3267,16 +3262,16 @@
         <v>80</v>
       </c>
       <c r="K9">
-        <v>34.907456000000003</v>
+        <v>12.800094</v>
       </c>
       <c r="L9">
-        <v>1317.315204</v>
+        <v>241.20740599999999</v>
       </c>
       <c r="M9">
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>3</v>
       </c>
@@ -3305,16 +3300,16 @@
         <v>90</v>
       </c>
       <c r="K10">
-        <v>52.141579</v>
+        <v>22.639842000000002</v>
       </c>
       <c r="L10">
-        <v>1232.531933</v>
+        <v>254.00538800000001</v>
       </c>
       <c r="M10">
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>3</v>
       </c>
@@ -3343,16 +3338,16 @@
         <v>100</v>
       </c>
       <c r="K11">
-        <v>65.303605000000005</v>
+        <v>18.587063000000001</v>
       </c>
       <c r="L11">
-        <v>1241.9451529999999</v>
+        <v>259.46514000000002</v>
       </c>
       <c r="M11">
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>3</v>
       </c>
@@ -3381,16 +3376,16 @@
         <v>110</v>
       </c>
       <c r="K12">
-        <v>100.469453</v>
+        <v>15.831378000000001</v>
       </c>
       <c r="L12">
-        <v>1244.0162190000001</v>
+        <v>256.45106199999998</v>
       </c>
       <c r="M12">
         <v>110</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>3</v>
       </c>
@@ -3419,16 +3414,16 @@
         <v>120</v>
       </c>
       <c r="K13">
-        <v>49.055357999999998</v>
+        <v>24.456137999999999</v>
       </c>
       <c r="L13">
-        <v>1260.781855</v>
+        <v>373.45311600000002</v>
       </c>
       <c r="M13">
         <v>120</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>3</v>
       </c>
@@ -3457,16 +3452,16 @@
         <v>130</v>
       </c>
       <c r="K14">
-        <v>63.487310999999998</v>
+        <v>18.024093000000001</v>
       </c>
       <c r="L14">
-        <v>1530.580285</v>
+        <v>298.67139100000003</v>
       </c>
       <c r="M14">
         <v>130</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>3</v>
       </c>
@@ -3495,16 +3490,16 @@
         <v>140</v>
       </c>
       <c r="K15">
-        <v>128.539466</v>
+        <v>22.389600999999999</v>
       </c>
       <c r="L15">
-        <v>1709.87247</v>
+        <v>498.03247299999998</v>
       </c>
       <c r="M15">
         <v>140</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>3</v>
       </c>
@@ -3533,10 +3528,10 @@
         <v>150</v>
       </c>
       <c r="K16">
-        <v>141.32024100000001</v>
+        <v>36.025244999999998</v>
       </c>
       <c r="L16">
-        <v>1713.2188960000001</v>
+        <v>363.73079100000001</v>
       </c>
       <c r="M16">
         <v>150</v>
@@ -3571,10 +3566,10 @@
         <v>160</v>
       </c>
       <c r="K17">
-        <v>191.37505999999999</v>
+        <v>39.111165</v>
       </c>
       <c r="L17">
-        <v>1299.587839</v>
+        <v>335.15546399999999</v>
       </c>
       <c r="M17">
         <v>160</v>
@@ -3609,10 +3604,10 @@
         <v>170</v>
       </c>
       <c r="K18">
-        <v>326.80600199999998</v>
+        <v>22.942609999999998</v>
       </c>
       <c r="L18">
-        <v>1657.974794</v>
+        <v>292.869933</v>
       </c>
       <c r="M18">
         <v>170</v>
@@ -3647,10 +3642,10 @@
         <v>180</v>
       </c>
       <c r="K19">
-        <v>366.15835399999997</v>
+        <v>37.693326999999996</v>
       </c>
       <c r="L19">
-        <v>1486.057665</v>
+        <v>288.34444000000002</v>
       </c>
       <c r="M19">
         <v>180</v>
@@ -3685,10 +3680,10 @@
         <v>190</v>
       </c>
       <c r="K20">
-        <v>440.23281900000001</v>
+        <v>57.586238999999999</v>
       </c>
       <c r="L20">
-        <v>2151.6544370000001</v>
+        <v>716.17199800000003</v>
       </c>
       <c r="M20">
         <v>190</v>
@@ -3723,10 +3718,10 @@
         <v>200</v>
       </c>
       <c r="K21">
-        <v>1087.4390390000001</v>
+        <v>74.960425999999998</v>
       </c>
       <c r="L21">
-        <v>2038.5303859999999</v>
+        <v>333.04666600000002</v>
       </c>
       <c r="M21">
         <v>200</v>
@@ -3761,10 +3756,10 @@
         <v>210</v>
       </c>
       <c r="K22">
-        <v>118.36072900000001</v>
+        <v>263.34917899999999</v>
       </c>
       <c r="L22">
-        <v>2832.1848540000001</v>
+        <v>1439.6864519999999</v>
       </c>
       <c r="M22">
         <v>210</v>
@@ -3799,10 +3794,10 @@
         <v>220</v>
       </c>
       <c r="K23">
-        <v>1518.6257009999999</v>
+        <v>102.681488</v>
       </c>
       <c r="L23">
-        <v>2279.2279490000001</v>
+        <v>2397.771002</v>
       </c>
       <c r="M23">
         <v>220</v>
@@ -3837,10 +3832,10 @@
         <v>230</v>
       </c>
       <c r="K24">
-        <v>839.83098299999995</v>
+        <v>214.71129500000001</v>
       </c>
       <c r="L24">
-        <v>3318.2705930000002</v>
+        <v>1876.7702609999999</v>
       </c>
       <c r="M24">
         <v>230</v>
@@ -3875,10 +3870,10 @@
         <v>240</v>
       </c>
       <c r="K25">
-        <v>566.17356700000005</v>
+        <v>370.14774299999999</v>
       </c>
       <c r="L25">
-        <v>3658.1806630000001</v>
+        <v>3361.3008140000002</v>
       </c>
       <c r="M25">
         <v>240</v>
@@ -3913,10 +3908,10 @@
         <v>250</v>
       </c>
       <c r="K26">
-        <v>704.65662199999997</v>
+        <v>51.258637999999998</v>
       </c>
       <c r="L26">
-        <v>4264.5928439999998</v>
+        <v>718.56665699999996</v>
       </c>
       <c r="M26">
         <v>250</v>
@@ -3951,10 +3946,10 @@
         <v>260</v>
       </c>
       <c r="K27">
-        <v>3103.9163990000002</v>
+        <v>402.48123399999997</v>
       </c>
       <c r="L27">
-        <v>6556.0165630000001</v>
+        <v>2124.5168720000001</v>
       </c>
       <c r="M27">
         <v>260</v>
@@ -3989,10 +3984,10 @@
         <v>270</v>
       </c>
       <c r="K28">
-        <v>8506.0341929999995</v>
+        <v>2347.0795589999998</v>
       </c>
       <c r="L28">
-        <v>6496.5461109999997</v>
+        <v>4635.1813030000003</v>
       </c>
       <c r="M28">
         <v>270</v>
@@ -4027,10 +4022,10 @@
         <v>280</v>
       </c>
       <c r="K29">
-        <v>13880.508502000001</v>
+        <v>74.959519999999998</v>
       </c>
       <c r="L29">
-        <v>12842.04996</v>
+        <v>5104.0190309999998</v>
       </c>
       <c r="M29">
         <v>280</v>
@@ -4055,6 +4050,24 @@
       <c r="F30">
         <v>1</v>
       </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>290</v>
+      </c>
+      <c r="J30">
+        <v>290</v>
+      </c>
+      <c r="K30">
+        <v>144.595731</v>
+      </c>
+      <c r="L30">
+        <v>7838.3213779999996</v>
+      </c>
+      <c r="M30">
+        <v>290</v>
+      </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31">
@@ -4074,6 +4087,24 @@
       </c>
       <c r="F31">
         <v>1</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>300</v>
+      </c>
+      <c r="J31">
+        <v>300</v>
+      </c>
+      <c r="K31">
+        <v>62.140711000000003</v>
+      </c>
+      <c r="L31">
+        <v>9029.3701259999998</v>
+      </c>
+      <c r="M31">
+        <v>300</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>